<commit_message>
Documentación nuevo modelo, cambios visualización imágenes de reporte
</commit_message>
<xml_diff>
--- a/detection_results.xlsx
+++ b/detection_results.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139">
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="154">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="155">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="156">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158">
@@ -2012,7 +2012,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="159">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164">
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="170">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173">
@@ -2162,7 +2162,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175">
@@ -2202,7 +2202,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181">
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -2252,7 +2252,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188">
@@ -2312,7 +2312,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="189">
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192">
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -2362,7 +2362,7 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -2402,7 +2402,7 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="198">
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202">
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -2462,7 +2462,7 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -2472,7 +2472,7 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="206">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222">
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="B223" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224">
@@ -2672,7 +2672,7 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225">
@@ -2692,7 +2692,7 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="227">
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="228">
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230">
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="235">
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236">
@@ -2792,7 +2792,7 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="237">
@@ -2802,7 +2802,7 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="241">
@@ -2852,7 +2852,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243">
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245">
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="247">
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="B250" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="251">
@@ -2942,7 +2942,7 @@
         </is>
       </c>
       <c r="B251" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="252">
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="B252" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="253">
@@ -2962,7 +2962,7 @@
         </is>
       </c>
       <c r="B253" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="254">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="B255" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="256">
@@ -3002,7 +3002,7 @@
         </is>
       </c>
       <c r="B257" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="258">
@@ -3012,7 +3012,7 @@
         </is>
       </c>
       <c r="B258" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="259">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="B259" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="260">
@@ -3032,7 +3032,7 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="261">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="B261" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="262">
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="263">
@@ -3062,7 +3062,7 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="264">
@@ -3072,7 +3072,7 @@
         </is>
       </c>
       <c r="B264" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="265">
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="B265" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="266">
@@ -3092,7 +3092,7 @@
         </is>
       </c>
       <c r="B266" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="267">
@@ -3102,7 +3102,7 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="268">
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="269">
@@ -3122,7 +3122,7 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="270">
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="B270" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="271">
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="272">
@@ -3152,7 +3152,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273">
@@ -3162,7 +3162,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="274">
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="275">
@@ -3212,7 +3212,7 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="279">
@@ -3222,7 +3222,7 @@
         </is>
       </c>
       <c r="B279" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="280">
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="B280" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="281">
@@ -3242,7 +3242,7 @@
         </is>
       </c>
       <c r="B281" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="282">
@@ -3252,7 +3252,7 @@
         </is>
       </c>
       <c r="B282" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283">
@@ -3272,7 +3272,7 @@
         </is>
       </c>
       <c r="B284" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="285">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="B286" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="287">
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="288">
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="B288" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="289">
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="290">
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="B290" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="291">
@@ -3352,7 +3352,7 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="293">
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="B297" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="298">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="301">
@@ -3452,7 +3452,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="303">
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="B303" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="304">
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="B306" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="307">
@@ -3502,7 +3502,7 @@
         </is>
       </c>
       <c r="B307" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="308">
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="309">
@@ -3522,7 +3522,7 @@
         </is>
       </c>
       <c r="B309" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="310">
@@ -3532,7 +3532,7 @@
         </is>
       </c>
       <c r="B310" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="311">
@@ -3562,7 +3562,7 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314">
@@ -3572,7 +3572,7 @@
         </is>
       </c>
       <c r="B314" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="315">
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="B315" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316">
@@ -3592,7 +3592,7 @@
         </is>
       </c>
       <c r="B316" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="317">
@@ -3602,7 +3602,7 @@
         </is>
       </c>
       <c r="B317" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="318">
@@ -3622,7 +3622,7 @@
         </is>
       </c>
       <c r="B319" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="320">
@@ -3732,7 +3732,7 @@
         </is>
       </c>
       <c r="B330" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="331">
@@ -3752,7 +3752,7 @@
         </is>
       </c>
       <c r="B332" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="333">
@@ -3762,7 +3762,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="334">
@@ -3772,7 +3772,7 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="335">
@@ -3782,7 +3782,7 @@
         </is>
       </c>
       <c r="B335" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="336">
@@ -3812,7 +3812,7 @@
         </is>
       </c>
       <c r="B338" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="339">
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="B339" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="340">
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="B340" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="341">
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="B342" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="343">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="B345" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="346">
@@ -3902,7 +3902,7 @@
         </is>
       </c>
       <c r="B347" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="348">
@@ -3922,7 +3922,7 @@
         </is>
       </c>
       <c r="B349" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="350">
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="B350" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="351">
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="B351" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="352">
@@ -3952,7 +3952,7 @@
         </is>
       </c>
       <c r="B352" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="353">
@@ -3972,7 +3972,7 @@
         </is>
       </c>
       <c r="B354" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355">
@@ -3992,7 +3992,7 @@
         </is>
       </c>
       <c r="B356" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="357">
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="B357" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="358">
@@ -4012,7 +4012,7 @@
         </is>
       </c>
       <c r="B358" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="359">
@@ -4022,7 +4022,7 @@
         </is>
       </c>
       <c r="B359" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="360">
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="B360" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="361">
@@ -4042,7 +4042,7 @@
         </is>
       </c>
       <c r="B361" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="362">
@@ -4062,7 +4062,7 @@
         </is>
       </c>
       <c r="B363" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="364">
@@ -4072,7 +4072,7 @@
         </is>
       </c>
       <c r="B364" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="365">
@@ -4082,7 +4082,7 @@
         </is>
       </c>
       <c r="B365" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="366">
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="B366" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="367">
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="B367" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="368">
@@ -4112,7 +4112,7 @@
         </is>
       </c>
       <c r="B368" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="369">
@@ -4122,7 +4122,7 @@
         </is>
       </c>
       <c r="B369" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="370">
@@ -4132,7 +4132,7 @@
         </is>
       </c>
       <c r="B370" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="371">
@@ -4142,7 +4142,7 @@
         </is>
       </c>
       <c r="B371" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372">
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="B372" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="373">
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="B374" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375">
@@ -4202,7 +4202,7 @@
         </is>
       </c>
       <c r="B377" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="378">
@@ -4212,7 +4212,7 @@
         </is>
       </c>
       <c r="B378" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="379">
@@ -4222,7 +4222,7 @@
         </is>
       </c>
       <c r="B379" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="380">
@@ -4232,7 +4232,7 @@
         </is>
       </c>
       <c r="B380" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="381">
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="B381" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="382">
@@ -4262,7 +4262,7 @@
         </is>
       </c>
       <c r="B383" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="384">
@@ -4272,7 +4272,7 @@
         </is>
       </c>
       <c r="B384" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385">
@@ -4282,7 +4282,7 @@
         </is>
       </c>
       <c r="B385" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386">
@@ -4312,7 +4312,7 @@
         </is>
       </c>
       <c r="B388" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="389">
@@ -4322,7 +4322,7 @@
         </is>
       </c>
       <c r="B389" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="390">
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="B390" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="391">
@@ -4342,7 +4342,7 @@
         </is>
       </c>
       <c r="B391" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="392">
@@ -4372,7 +4372,7 @@
         </is>
       </c>
       <c r="B394" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="395">
@@ -4402,7 +4402,7 @@
         </is>
       </c>
       <c r="B397" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="398">
@@ -4412,7 +4412,7 @@
         </is>
       </c>
       <c r="B398" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="399">
@@ -4462,7 +4462,7 @@
         </is>
       </c>
       <c r="B403" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="404">
@@ -4482,7 +4482,7 @@
         </is>
       </c>
       <c r="B405" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="406">
@@ -4512,7 +4512,7 @@
         </is>
       </c>
       <c r="B408" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="409">
@@ -4522,7 +4522,7 @@
         </is>
       </c>
       <c r="B409" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="410">
@@ -4532,7 +4532,7 @@
         </is>
       </c>
       <c r="B410" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="411">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="B411" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="412">
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="B412" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="413">
@@ -4562,7 +4562,7 @@
         </is>
       </c>
       <c r="B413" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="414">
@@ -4572,7 +4572,7 @@
         </is>
       </c>
       <c r="B414" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="415">
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="B416" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="417">
@@ -4602,7 +4602,7 @@
         </is>
       </c>
       <c r="B417" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="418">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="B418" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="419">
@@ -4622,7 +4622,7 @@
         </is>
       </c>
       <c r="B419" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="420">
@@ -4642,7 +4642,7 @@
         </is>
       </c>
       <c r="B421" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="422">
@@ -4662,7 +4662,7 @@
         </is>
       </c>
       <c r="B423" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="424">
@@ -4682,7 +4682,7 @@
         </is>
       </c>
       <c r="B425" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="426">
@@ -4712,7 +4712,7 @@
         </is>
       </c>
       <c r="B428" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="429">
@@ -4722,7 +4722,7 @@
         </is>
       </c>
       <c r="B429" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="430">
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="B430" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="431">
@@ -4742,7 +4742,7 @@
         </is>
       </c>
       <c r="B431" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="432">
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="B435" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="436">
@@ -4792,7 +4792,7 @@
         </is>
       </c>
       <c r="B436" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="437">
@@ -4802,7 +4802,7 @@
         </is>
       </c>
       <c r="B437" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="438">
@@ -4812,7 +4812,7 @@
         </is>
       </c>
       <c r="B438" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="439">
@@ -4822,7 +4822,7 @@
         </is>
       </c>
       <c r="B439" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="440">
@@ -4842,7 +4842,7 @@
         </is>
       </c>
       <c r="B441" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="442">
@@ -4852,7 +4852,7 @@
         </is>
       </c>
       <c r="B442" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="443">
@@ -4862,7 +4862,7 @@
         </is>
       </c>
       <c r="B443" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="444">
@@ -4872,7 +4872,7 @@
         </is>
       </c>
       <c r="B444" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="445">
@@ -4882,7 +4882,7 @@
         </is>
       </c>
       <c r="B445" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="446">
@@ -4892,7 +4892,7 @@
         </is>
       </c>
       <c r="B446" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="447">
@@ -4912,7 +4912,7 @@
         </is>
       </c>
       <c r="B448" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="449">
@@ -4922,7 +4922,7 @@
         </is>
       </c>
       <c r="B449" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="450">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="B450" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="451">
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="B451" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="452">
@@ -4952,7 +4952,7 @@
         </is>
       </c>
       <c r="B452" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="453">
@@ -4962,7 +4962,7 @@
         </is>
       </c>
       <c r="B453" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="454">
@@ -4972,7 +4972,7 @@
         </is>
       </c>
       <c r="B454" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="455">
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="B455" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="456">
@@ -4992,7 +4992,7 @@
         </is>
       </c>
       <c r="B456" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="457">
@@ -5002,7 +5002,7 @@
         </is>
       </c>
       <c r="B457" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="458">
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="B458" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="459">
@@ -5022,7 +5022,7 @@
         </is>
       </c>
       <c r="B459" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="460">
@@ -5052,7 +5052,7 @@
         </is>
       </c>
       <c r="B462" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="463">
@@ -5062,7 +5062,7 @@
         </is>
       </c>
       <c r="B463" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="464">
@@ -5072,7 +5072,7 @@
         </is>
       </c>
       <c r="B464" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="465">
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="B465" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="466">
@@ -5092,7 +5092,7 @@
         </is>
       </c>
       <c r="B466" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="467">
@@ -5102,7 +5102,7 @@
         </is>
       </c>
       <c r="B467" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="468">
@@ -5112,7 +5112,7 @@
         </is>
       </c>
       <c r="B468" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="469">
@@ -5142,7 +5142,7 @@
         </is>
       </c>
       <c r="B471" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="472">
@@ -5152,7 +5152,7 @@
         </is>
       </c>
       <c r="B472" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="473">
@@ -5162,7 +5162,7 @@
         </is>
       </c>
       <c r="B473" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="474">
@@ -5172,7 +5172,7 @@
         </is>
       </c>
       <c r="B474" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="475">
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="B475" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="476">
@@ -5192,7 +5192,7 @@
         </is>
       </c>
       <c r="B476" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="477">
@@ -5202,7 +5202,7 @@
         </is>
       </c>
       <c r="B477" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="478">
@@ -5212,7 +5212,7 @@
         </is>
       </c>
       <c r="B478" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="479">
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="B479" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="480">
@@ -5232,7 +5232,7 @@
         </is>
       </c>
       <c r="B480" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="481">
@@ -5242,7 +5242,7 @@
         </is>
       </c>
       <c r="B481" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="482">
@@ -5282,7 +5282,7 @@
         </is>
       </c>
       <c r="B485" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486">
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="B486" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="487">
@@ -5312,7 +5312,7 @@
         </is>
       </c>
       <c r="B488" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="489">
@@ -5322,7 +5322,7 @@
         </is>
       </c>
       <c r="B489" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="490">
@@ -5362,7 +5362,7 @@
         </is>
       </c>
       <c r="B493" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="494">
@@ -5382,7 +5382,7 @@
         </is>
       </c>
       <c r="B495" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="496">
@@ -5402,7 +5402,7 @@
         </is>
       </c>
       <c r="B497" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="498">
@@ -5412,7 +5412,7 @@
         </is>
       </c>
       <c r="B498" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="499">
@@ -5422,7 +5422,7 @@
         </is>
       </c>
       <c r="B499" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="500">
@@ -5432,7 +5432,7 @@
         </is>
       </c>
       <c r="B500" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="501">
@@ -5442,7 +5442,7 @@
         </is>
       </c>
       <c r="B501" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="502">
@@ -5452,7 +5452,7 @@
         </is>
       </c>
       <c r="B502" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="503">
@@ -5462,7 +5462,7 @@
         </is>
       </c>
       <c r="B503" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="504">
@@ -5472,7 +5472,7 @@
         </is>
       </c>
       <c r="B504" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="505">
@@ -5482,7 +5482,7 @@
         </is>
       </c>
       <c r="B505" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="506">
@@ -5492,7 +5492,7 @@
         </is>
       </c>
       <c r="B506" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="507">
@@ -5502,7 +5502,7 @@
         </is>
       </c>
       <c r="B507" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="508">
@@ -5512,7 +5512,7 @@
         </is>
       </c>
       <c r="B508" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="509">
@@ -5542,7 +5542,7 @@
         </is>
       </c>
       <c r="B511" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="512">
@@ -5562,7 +5562,7 @@
         </is>
       </c>
       <c r="B513" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="514">
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="B514" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="515">
@@ -5602,7 +5602,7 @@
         </is>
       </c>
       <c r="B517" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="518">
@@ -5612,7 +5612,7 @@
         </is>
       </c>
       <c r="B518" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="519">
@@ -5622,7 +5622,7 @@
         </is>
       </c>
       <c r="B519" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="520">
@@ -5632,7 +5632,7 @@
         </is>
       </c>
       <c r="B520" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="521">
@@ -5682,7 +5682,7 @@
         </is>
       </c>
       <c r="B525" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="526">
@@ -5702,7 +5702,7 @@
         </is>
       </c>
       <c r="B527" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="528">
@@ -5962,7 +5962,7 @@
         </is>
       </c>
       <c r="B553" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="554">

</xml_diff>